<commit_message>
readme updates, final slides, etc
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\CIS565 GPU Programming\Project5-Particle-Filter-SLAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\CIS565 GPU Programming\FinalProject-FastSLAM - PCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="10755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="10755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="occupancygrid" sheetId="1" r:id="rId1"/>
+    <sheet name="pointcloud" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Improvement</t>
   </si>
@@ -63,6 +64,61 @@
   </si>
   <si>
     <t>LIDAR</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Framerate Start</t>
+  </si>
+  <si>
+    <t>Framerate End</t>
+  </si>
+  <si>
+    <t>with balance</t>
+  </si>
+  <si>
+    <t>don't check free cells</t>
+  </si>
+  <si>
+    <t>kernEvaluateParticles ~300 us</t>
+  </si>
+  <si>
+    <t>Map with thrust:</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Occupancy Grid
+(us)</t>
+  </si>
+  <si>
+    <t>Point Cloud
+(us)</t>
+  </si>
+  <si>
+    <t>Dynamic
+Measurement Kernel</t>
+  </si>
+  <si>
+    <t>GPU Map Update</t>
+  </si>
+  <si>
+    <t>Time
+(us)</t>
+  </si>
+  <si>
+    <t>No Regression Fit</t>
+  </si>
+  <si>
+    <t>KD Tree Balancing</t>
+  </si>
+  <si>
+    <t>particles</t>
+  </si>
+  <si>
+    <t>Hz</t>
   </si>
 </sst>
 </file>
@@ -125,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -146,6 +202,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,7 +322,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>occupancygrid!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -279,7 +357,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>occupancygrid!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -306,7 +384,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>occupancygrid!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -343,7 +421,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>occupancygrid!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -378,7 +456,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>occupancygrid!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -405,7 +483,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>occupancygrid!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -442,7 +520,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>occupancygrid!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -466,7 +544,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>occupancygrid!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -493,7 +571,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>occupancygrid!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1726,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="E1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,4 +2025,321 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B3">
+        <v>14.2</v>
+      </c>
+      <c r="C3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5</v>
+      </c>
+      <c r="J3" s="2">
+        <f>I3/H3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.05</v>
+      </c>
+      <c r="B4" s="9">
+        <v>15.6</v>
+      </c>
+      <c r="C4">
+        <v>10.1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <v>40</v>
+      </c>
+      <c r="I4" s="3">
+        <v>510</v>
+      </c>
+      <c r="J4" s="3">
+        <f>I4/H4</f>
+        <v>12.75</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>85</v>
+      </c>
+      <c r="J5" s="2">
+        <f>I5/H5</f>
+        <v>17</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="7">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7">
+        <f>I6/H6</f>
+        <v>0.25</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B7">
+        <v>13.4</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <f>SUM(H3:H6)</f>
+        <v>70</v>
+      </c>
+      <c r="I7" s="2">
+        <f>SUM(I3:I6)</f>
+        <v>605</v>
+      </c>
+      <c r="J7" s="2">
+        <f>I7/H7</f>
+        <v>8.6428571428571423</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+      <c r="N12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+      <c r="N13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="13">
+        <v>105</v>
+      </c>
+      <c r="P13" s="13">
+        <f>I4/O13</f>
+        <v>4.8571428571428568</v>
+      </c>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+      <c r="N14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="14">
+        <v>510</v>
+      </c>
+      <c r="P14" s="16">
+        <f>I4/O14</f>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="2">
+        <v>415</v>
+      </c>
+      <c r="P15" s="13">
+        <f>I4/O15</f>
+        <v>1.2289156626506024</v>
+      </c>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="7">
+        <v>215</v>
+      </c>
+      <c r="P16" s="15">
+        <f>I5/O16</f>
+        <v>0.39534883720930231</v>
+      </c>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>500</v>
+      </c>
+      <c r="B18">
+        <v>16.5</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5000</v>
+      </c>
+      <c r="B19">
+        <v>1.2</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>